<commit_message>
updated matlab.xlsx with cvg test results
</commit_message>
<xml_diff>
--- a/hw5/matlab.xlsx
+++ b/hw5/matlab.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>CG Method</t>
   </si>
@@ -118,6 +117,15 @@
   </si>
   <si>
     <t>32g</t>
+  </si>
+  <si>
+    <t>u-uh</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>iter</t>
   </si>
 </sst>
 </file>
@@ -440,14 +448,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
   </cols>
@@ -949,7 +958,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>18</v>
       </c>
@@ -960,7 +969,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -969,6 +978,181 @@
       </c>
       <c r="C34" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>32</v>
+      </c>
+      <c r="B38">
+        <f>0.00301277655464715</f>
+        <v>3.0127765546471498E-3</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1.22599601745605E-2</v>
+      </c>
+      <c r="D38">
+        <v>48</v>
+      </c>
+      <c r="E38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>64</v>
+      </c>
+      <c r="B39" s="1">
+        <v>7.7810619700602302E-4</v>
+      </c>
+      <c r="C39" s="1">
+        <v>2.9861927032470699E-3</v>
+      </c>
+      <c r="D39">
+        <v>96</v>
+      </c>
+      <c r="E39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>128</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1.9764834769608799E-4</v>
+      </c>
+      <c r="C40" s="1">
+        <v>3.2128095626830999E-2</v>
+      </c>
+      <c r="D40">
+        <v>192</v>
+      </c>
+      <c r="E40" s="1">
+        <f>B39/B40</f>
+        <v>3.9368211577587799</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>256</v>
+      </c>
+      <c r="B41" s="1">
+        <v>4.9797438583243302E-5</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0.16878199577331501</v>
+      </c>
+      <c r="D41">
+        <v>387</v>
+      </c>
+      <c r="E41" s="1">
+        <f t="shared" ref="E41:E48" si="3">B40/B41</f>
+        <v>3.969046467434092</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>512</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1.24942786493553E-5</v>
+      </c>
+      <c r="C42" s="1">
+        <v>1.2435050010681099</v>
+      </c>
+      <c r="D42">
+        <v>783</v>
+      </c>
+      <c r="E42" s="1">
+        <f t="shared" si="3"/>
+        <v>3.985619336720398</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1024</v>
+      </c>
+      <c r="B43" s="1">
+        <v>3.1266064489665598E-6</v>
+      </c>
+      <c r="C43" s="1">
+        <v>12.432227849960301</v>
+      </c>
+      <c r="D43">
+        <v>1581</v>
+      </c>
+      <c r="E43" s="1">
+        <f t="shared" si="3"/>
+        <v>3.996114910299966</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>2048</v>
+      </c>
+      <c r="B44" s="1">
+        <v>7.8019385341132598E-7</v>
+      </c>
+      <c r="C44" s="1">
+        <v>124.338080883026</v>
+      </c>
+      <c r="D44">
+        <v>3192</v>
+      </c>
+      <c r="E44" s="1">
+        <f t="shared" si="3"/>
+        <v>4.0074738288385126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>4096</v>
+      </c>
+      <c r="E45" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>8162</v>
+      </c>
+      <c r="E46" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>16384</v>
+      </c>
+      <c r="E47" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>32768</v>
+      </c>
+      <c r="E48" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>